<commit_message>
CHANGE:NuevasCarpetas y estructura de archivos
</commit_message>
<xml_diff>
--- a/data/raw/Datos_Abiertos_ARESEP_Tarifas_de_electricidad_del_sistema_de_distribución_2015.xlsx
+++ b/data/raw/Datos_Abiertos_ARESEP_Tarifas_de_electricidad_del_sistema_de_distribución_2015.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fab_t\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97212ba63cabc353/CUC/PrograII/Proyecto5_Predicción_delConsumode_EnergíaenCostaRica/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8477A178-32A4-4D60-B1FD-F845474C77A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8477A178-32A4-4D60-B1FD-F845474C77A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEE8965A-AF5C-4976-9B7A-B89A187091AC}"/>
   <bookViews>
-    <workbookView xWindow="15570" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13230" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -265,6 +265,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -556,9 +560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>